<commit_message>
add sample data raw in bulk upload account details
</commit_message>
<xml_diff>
--- a/public/Sample file.xlsx
+++ b/public/Sample file.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
   <si>
     <t xml:space="preserve">Client Id</t>
   </si>
@@ -55,7 +55,7 @@
     <t xml:space="preserve">PABS Duties</t>
   </si>
   <si>
-    <t xml:space="preserve">Bookkeeping Monthly or Clean Up (Period – Months/Years)</t>
+    <t xml:space="preserve">Bookkeeping Monthly/Clean up catch up (Specify Period)</t>
   </si>
   <si>
     <t xml:space="preserve">Deadline</t>
@@ -65,14 +65,58 @@
   </si>
   <si>
     <t xml:space="preserve">Notes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AAA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">XYZ Company</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Residential Construction</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Real Estate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Scorp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">QBO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dropbox</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Yes or No</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cash or Accruals</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Categorize (Put checks in Misc)
+2. Reconcile Bank Account (1 bank)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">catch up for 2021</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bank account transactions 170
+Journal entries 2
+Bank deposits 12
+Expenses 158	</t>
+  </si>
+  <si>
+    <t xml:space="preserve">XYZ</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="General"/>
+    <numFmt numFmtId="165" formatCode="dd/mm/yy"/>
   </numFmts>
   <fonts count="5">
     <font>
@@ -161,13 +205,21 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -247,13 +299,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:O1"/>
+  <dimension ref="A1:O2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="N7" activeCellId="0" sqref="N7"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="J1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="N9" activeCellId="0" sqref="N9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="32.30078125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="32.32421875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="8.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="17.85"/>
@@ -265,7 +317,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="30.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="25.72"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="22.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="11.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="30.53"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="32"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="9"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="28.42"/>
@@ -317,6 +369,53 @@
       </c>
       <c r="O1" s="1" t="s">
         <v>14</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="D2" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="E2" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="F2" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="G2" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="H2" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="I2" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="J2" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="L2" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="M2" s="3" t="n">
+        <v>45451</v>
+      </c>
+      <c r="N2" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="O2" s="0" t="s">
+        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>